<commit_message>
Summary of factor load decisions
</commit_message>
<xml_diff>
--- a/2010/hacking/FamaFrench/data/output/spreadsheets/BRSIX_regression.xlsx
+++ b/2010/hacking/FamaFrench/data/output/spreadsheets/BRSIX_regression.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="16275" windowHeight="11820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="22410" windowHeight="13545"/>
   </bookViews>
   <sheets>
     <sheet name="BRSIX_regression" sheetId="1" r:id="rId1"/>
     <sheet name="last 5 years" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:T43"/>
 </workbook>
 </file>
 
@@ -1393,7 +1394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
@@ -5188,7 +5189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4:S26"/>
     </sheetView>
   </sheetViews>

</xml_diff>